<commit_message>
Tuan - added the Workload.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Workload.xlsx
+++ b/Documents/Workload.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Preprocessing</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>Minh</t>
+  </si>
+  <si>
+    <t>Centroid</t>
+  </si>
+  <si>
+    <t>Compactness</t>
+  </si>
+  <si>
+    <t>Moment</t>
+  </si>
+  <si>
+    <t>Nearest Neighbour</t>
+  </si>
+  <si>
+    <t>SVM</t>
   </si>
 </sst>
 </file>
@@ -439,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,15 +616,55 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>